<commit_message>
Added new required columns to NWSS output, including epaid id, pasteurization, and some lab metadata fields.
</commit_message>
<xml_diff>
--- a/analysis/resources/WaTCH_to_NWSS.xlsx
+++ b/analysis/resources/WaTCH_to_NWSS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/Dropbox (DriscollMML)/Project_WaTCH/ANALYSIS/RESOURCES/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/analysis/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A0E239-082C-AB45-9B32-74891D331868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC93157-7CDE-9949-A4C4-4C47943F0FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{8B6D7199-4C21-CD4F-9BF8-C2C00BB87A59}"/>
+    <workbookView xWindow="33140" yWindow="1560" windowWidth="29360" windowHeight="18180" xr2:uid="{8B6D7199-4C21-CD4F-9BF8-C2C00BB87A59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="107">
   <si>
     <t>reporting_jurisdiction</t>
   </si>
@@ -334,6 +334,27 @@
   </si>
   <si>
     <t>pcr_target_units</t>
+  </si>
+  <si>
+    <t>epaid</t>
+  </si>
+  <si>
+    <t>pasteurized</t>
+  </si>
+  <si>
+    <t>pretreatment</t>
+  </si>
+  <si>
+    <t>major_lab_method</t>
+  </si>
+  <si>
+    <t>major_lab_method_desc</t>
+  </si>
+  <si>
+    <t>epaid_id</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -724,11 +745,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B147B1-E705-4D4E-A6A3-C9D149CC035A}">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1252,10 +1273,58 @@
         <v>35</v>
       </c>
     </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>105</v>
+      </c>
+      <c r="B42" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" t="s">
+        <v>101</v>
+      </c>
+      <c r="D43" t="s">
+        <v>106</v>
+      </c>
+    </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
+      <c r="A44" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" t="s">
+        <v>102</v>
+      </c>
       <c r="C44" s="4"/>
+      <c r="D44" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" t="s">
+        <v>103</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" t="s">
+        <v>104</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added NWSS site_id field generation to the DAP.
</commit_message>
<xml_diff>
--- a/analysis/resources/WaTCH_to_NWSS.xlsx
+++ b/analysis/resources/WaTCH_to_NWSS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/analysis/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC93157-7CDE-9949-A4C4-4C47943F0FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9E0BB3-464E-684F-9F44-E3335B040895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33140" yWindow="1560" windowWidth="29360" windowHeight="18180" xr2:uid="{8B6D7199-4C21-CD4F-9BF8-C2C00BB87A59}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="109">
   <si>
     <t>reporting_jurisdiction</t>
   </si>
@@ -355,6 +355,12 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>site_id</t>
+  </si>
+  <si>
+    <t>nwss_site_id</t>
   </si>
 </sst>
 </file>
@@ -745,11 +751,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B147B1-E705-4D4E-A6A3-C9D149CC035A}">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A37" sqref="A37:XFD37"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1326,6 +1332,17 @@
         <v>104</v>
       </c>
     </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>108</v>
+      </c>
+      <c r="B47" t="s">
+        <v>107</v>
+      </c>
+      <c r="C47" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>